<commit_message>
[19127478] import data to excel
</commit_message>
<xml_diff>
--- a/BookStore/window_data.xlsx
+++ b/BookStore/window_data.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\project 1\BookStore\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9423A2E1-3D33-470A-AB9C-D5C7BEBC6777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Truyện ngắn" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Tâm lý" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Kỹ năng" sheetId="3" r:id="rId6"/>
+    <sheet name="Short Story" sheetId="1" r:id="rId1"/>
+    <sheet name="Psychology" sheetId="2" r:id="rId2"/>
+    <sheet name="Skill" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -408,41 +417,42 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF242424"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF444444"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF242424"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF444444"/>
       <name val="Roboto"/>
     </font>
@@ -452,83 +462,74 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -718,27 +719,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B3:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="46.63"/>
-    <col customWidth="1" min="4" max="4" width="20.63"/>
-    <col customWidth="1" min="5" max="5" width="22.63"/>
-    <col customWidth="1" min="6" max="6" width="23.63"/>
-    <col customWidth="1" min="9" max="9" width="15.63"/>
+    <col min="3" max="3" width="46.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -767,9 +773,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
@@ -778,27 +784,27 @@
         <v>10</v>
       </c>
       <c r="E4" s="2">
-        <v>1988.0</v>
+        <v>1988</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="3">
-        <v>20000.0</v>
+        <v>20000</v>
       </c>
       <c r="H4" s="3">
-        <v>35000.0</v>
+        <v>35000</v>
       </c>
       <c r="I4" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J4" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
@@ -807,27 +813,27 @@
         <v>13</v>
       </c>
       <c r="E5" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="3">
-        <v>250000.0</v>
+        <v>250000</v>
       </c>
       <c r="H5" s="3">
-        <v>455000.0</v>
+        <v>455000</v>
       </c>
       <c r="I5" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J5" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -836,27 +842,27 @@
         <v>16</v>
       </c>
       <c r="E6" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="3">
-        <v>20000.0</v>
+        <v>20000</v>
       </c>
       <c r="H6" s="3">
-        <v>51000.0</v>
+        <v>51000</v>
       </c>
       <c r="I6" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J6" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>18</v>
@@ -865,27 +871,27 @@
         <v>19</v>
       </c>
       <c r="E7" s="2">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="3">
-        <v>35000.0</v>
+        <v>35000</v>
       </c>
       <c r="H7" s="3">
-        <v>84000.0</v>
+        <v>84000</v>
       </c>
       <c r="I7" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J7" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>21</v>
@@ -894,27 +900,27 @@
         <v>22</v>
       </c>
       <c r="E8" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="3">
-        <v>32000.0</v>
+        <v>32000</v>
       </c>
       <c r="H8" s="3">
-        <v>75000.0</v>
+        <v>75000</v>
       </c>
       <c r="I8" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J8" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>24</v>
@@ -923,27 +929,27 @@
         <v>25</v>
       </c>
       <c r="E9" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G9" s="3">
-        <v>41000.0</v>
+        <v>41000</v>
       </c>
       <c r="H9" s="3">
-        <v>57000.0</v>
+        <v>57000</v>
       </c>
       <c r="I9" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J9" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>27</v>
@@ -952,27 +958,27 @@
         <v>28</v>
       </c>
       <c r="E10" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G10" s="3">
-        <v>28000.0</v>
+        <v>28000</v>
       </c>
       <c r="H10" s="3">
-        <v>65000.0</v>
+        <v>65000</v>
       </c>
       <c r="I10" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J10" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>30</v>
@@ -981,27 +987,27 @@
         <v>31</v>
       </c>
       <c r="E11" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G11" s="3">
-        <v>50000.0</v>
+        <v>50000</v>
       </c>
       <c r="H11" s="3">
-        <v>72000.0</v>
+        <v>72000</v>
       </c>
       <c r="I11" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J11" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>33</v>
@@ -1010,27 +1016,27 @@
         <v>34</v>
       </c>
       <c r="E12" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="3">
-        <v>31000.0</v>
+        <v>31000</v>
       </c>
       <c r="H12" s="3">
-        <v>61000.0</v>
+        <v>61000</v>
       </c>
       <c r="I12" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J12" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>36</v>
@@ -1039,27 +1045,27 @@
         <v>37</v>
       </c>
       <c r="E13" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="3">
-        <v>16000.0</v>
+        <v>16000</v>
       </c>
       <c r="H13" s="3">
-        <v>36000.0</v>
+        <v>36000</v>
       </c>
       <c r="I13" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J13" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>38</v>
@@ -1068,27 +1074,27 @@
         <v>39</v>
       </c>
       <c r="E14" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G14" s="3">
-        <v>87000.0</v>
+        <v>87000</v>
       </c>
       <c r="H14" s="3">
-        <v>177000.0</v>
+        <v>177000</v>
       </c>
       <c r="I14" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J14" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>40</v>
@@ -1097,27 +1103,27 @@
         <v>41</v>
       </c>
       <c r="E15" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G15" s="3">
-        <v>43000.0</v>
+        <v>43000</v>
       </c>
       <c r="H15" s="3">
-        <v>89000.0</v>
+        <v>89000</v>
       </c>
       <c r="I15" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J15" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>42</v>
@@ -1126,27 +1132,27 @@
         <v>43</v>
       </c>
       <c r="E16" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G16" s="3">
-        <v>36000.0</v>
+        <v>36000</v>
       </c>
       <c r="H16" s="3">
-        <v>92000.0</v>
+        <v>92000</v>
       </c>
       <c r="I16" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J16" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>45</v>
@@ -1155,27 +1161,27 @@
         <v>22</v>
       </c>
       <c r="E17" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="3">
-        <v>25000.0</v>
+        <v>25000</v>
       </c>
       <c r="H17" s="3">
-        <v>59000.0</v>
+        <v>59000</v>
       </c>
       <c r="I17" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J17" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>46</v>
@@ -1184,27 +1190,27 @@
         <v>47</v>
       </c>
       <c r="E18" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G18" s="3">
-        <v>26000.0</v>
+        <v>26000</v>
       </c>
       <c r="H18" s="3">
-        <v>76000.0</v>
+        <v>76000</v>
       </c>
       <c r="I18" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J18" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>49</v>
@@ -1213,27 +1219,27 @@
         <v>50</v>
       </c>
       <c r="E19" s="6">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G19" s="3">
-        <v>47000.0</v>
+        <v>47000</v>
       </c>
       <c r="H19" s="3">
-        <v>73000.0</v>
+        <v>73000</v>
       </c>
       <c r="I19" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J19" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>52</v>
@@ -1242,27 +1248,27 @@
         <v>53</v>
       </c>
       <c r="E20" s="2">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G20" s="3">
-        <v>49000.0</v>
+        <v>49000</v>
       </c>
       <c r="H20" s="3">
-        <v>59000.0</v>
+        <v>59000</v>
       </c>
       <c r="I20" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J20" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>54</v>
@@ -1271,27 +1277,27 @@
         <v>55</v>
       </c>
       <c r="E21" s="2">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G21" s="3">
-        <v>37000.0</v>
+        <v>37000</v>
       </c>
       <c r="H21" s="3">
-        <v>99000.0</v>
+        <v>99000</v>
       </c>
       <c r="I21" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J21" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>56</v>
@@ -1300,27 +1306,27 @@
         <v>57</v>
       </c>
       <c r="E22" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="3">
-        <v>27000.0</v>
+        <v>27000</v>
       </c>
       <c r="H22" s="3">
-        <v>50000.0</v>
+        <v>50000</v>
       </c>
       <c r="I22" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J22" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>58</v>
@@ -1329,27 +1335,27 @@
         <v>59</v>
       </c>
       <c r="E23" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G23" s="3">
-        <v>38000.0</v>
+        <v>38000</v>
       </c>
       <c r="H23" s="3">
-        <v>51000.0</v>
+        <v>51000</v>
       </c>
       <c r="I23" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J23" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>60</v>
@@ -1358,27 +1364,27 @@
         <v>61</v>
       </c>
       <c r="E24" s="2">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G24" s="3">
-        <v>67000.0</v>
+        <v>67000</v>
       </c>
       <c r="H24" s="3">
-        <v>104000.0</v>
+        <v>104000</v>
       </c>
       <c r="I24" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J24" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>62</v>
@@ -1387,47 +1393,48 @@
         <v>63</v>
       </c>
       <c r="E25" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G25" s="3">
-        <v>128000.0</v>
+        <v>128000</v>
       </c>
       <c r="H25" s="3">
-        <v>378000.0</v>
+        <v>378000</v>
       </c>
       <c r="I25" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J25" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B3:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="61.63"/>
-    <col customWidth="1" min="4" max="4" width="14.75"/>
-    <col customWidth="1" min="6" max="6" width="21.5"/>
-    <col customWidth="1" min="9" max="9" width="16.0"/>
-    <col customWidth="1" min="10" max="10" width="14.75"/>
+    <col min="3" max="3" width="61.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3">
+    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
@@ -1456,9 +1463,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>64</v>
@@ -1467,27 +1474,27 @@
         <v>65</v>
       </c>
       <c r="E4" s="2">
-        <v>1988.0</v>
+        <v>1988</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="3">
-        <v>35000.0</v>
+        <v>35000</v>
       </c>
       <c r="H4" s="3">
-        <v>98000.0</v>
+        <v>98000</v>
       </c>
       <c r="I4" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J4" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>66</v>
@@ -1496,27 +1503,27 @@
         <v>67</v>
       </c>
       <c r="E5" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G5" s="3">
-        <v>20000.0</v>
+        <v>20000</v>
       </c>
       <c r="H5" s="3">
-        <v>45000.0</v>
+        <v>45000</v>
       </c>
       <c r="I5" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J5" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>68</v>
@@ -1525,27 +1532,27 @@
         <v>69</v>
       </c>
       <c r="E6" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="3">
-        <v>42000.0</v>
+        <v>42000</v>
       </c>
       <c r="H6" s="3">
-        <v>125000.0</v>
+        <v>125000</v>
       </c>
       <c r="I6" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J6" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>70</v>
@@ -1554,27 +1561,27 @@
         <v>71</v>
       </c>
       <c r="E7" s="2">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="3">
-        <v>80000.0</v>
+        <v>80000</v>
       </c>
       <c r="H7" s="3">
-        <v>235000.0</v>
+        <v>235000</v>
       </c>
       <c r="I7" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J7" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>72</v>
@@ -1583,27 +1590,27 @@
         <v>73</v>
       </c>
       <c r="E8" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="3">
-        <v>28000.0</v>
+        <v>28000</v>
       </c>
       <c r="H8" s="3">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I8" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J8" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="10">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>74</v>
@@ -1612,27 +1619,27 @@
         <v>75</v>
       </c>
       <c r="E9" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G9" s="3">
-        <v>46000.0</v>
+        <v>46000</v>
       </c>
       <c r="H9" s="3">
-        <v>159000.0</v>
+        <v>159000</v>
       </c>
       <c r="I9" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J9" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="10">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>76</v>
@@ -1641,27 +1648,27 @@
         <v>77</v>
       </c>
       <c r="E10" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G10" s="3">
-        <v>31000.0</v>
+        <v>31000</v>
       </c>
       <c r="H10" s="3">
-        <v>74000.0</v>
+        <v>74000</v>
       </c>
       <c r="I10" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J10" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="10">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>78</v>
@@ -1670,27 +1677,27 @@
         <v>79</v>
       </c>
       <c r="E11" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G11" s="3">
-        <v>43000.0</v>
+        <v>43000</v>
       </c>
       <c r="H11" s="3">
-        <v>129000.0</v>
+        <v>129000</v>
       </c>
       <c r="I11" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J11" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>80</v>
@@ -1699,27 +1706,27 @@
         <v>81</v>
       </c>
       <c r="E12" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="3">
-        <v>34000.0</v>
+        <v>34000</v>
       </c>
       <c r="H12" s="3">
-        <v>76000.0</v>
+        <v>76000</v>
       </c>
       <c r="I12" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J12" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>82</v>
@@ -1728,27 +1735,27 @@
         <v>83</v>
       </c>
       <c r="E13" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G13" s="3">
-        <v>37000.0</v>
+        <v>37000</v>
       </c>
       <c r="H13" s="3">
-        <v>102000.0</v>
+        <v>102000</v>
       </c>
       <c r="I13" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J13" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>84</v>
@@ -1757,27 +1764,27 @@
         <v>85</v>
       </c>
       <c r="E14" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G14" s="3">
-        <v>24000.0</v>
+        <v>24000</v>
       </c>
       <c r="H14" s="3">
-        <v>47000.0</v>
+        <v>47000</v>
       </c>
       <c r="I14" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J14" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="10">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>86</v>
@@ -1786,27 +1793,27 @@
         <v>87</v>
       </c>
       <c r="E15" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G15" s="3">
-        <v>30000.0</v>
+        <v>30000</v>
       </c>
       <c r="H15" s="3">
-        <v>74000.0</v>
+        <v>74000</v>
       </c>
       <c r="I15" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J15" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="10">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>88</v>
@@ -1815,46 +1822,47 @@
         <v>85</v>
       </c>
       <c r="E16" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G16" s="3">
-        <v>39000.0</v>
+        <v>39000</v>
       </c>
       <c r="H16" s="3">
-        <v>95000.0</v>
+        <v>95000</v>
       </c>
       <c r="I16" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J16" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B3:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="42.0"/>
-    <col customWidth="1" min="5" max="5" width="24.5"/>
-    <col customWidth="1" min="6" max="6" width="19.38"/>
-    <col customWidth="1" min="9" max="9" width="15.25"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3">
+    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
@@ -1883,9 +1891,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>89</v>
@@ -1894,27 +1902,27 @@
         <v>90</v>
       </c>
       <c r="E4" s="2">
-        <v>1988.0</v>
+        <v>1988</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="3">
-        <v>25000.0</v>
+        <v>25000</v>
       </c>
       <c r="H4" s="3">
-        <v>67000.0</v>
+        <v>67000</v>
       </c>
       <c r="I4" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J4" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>91</v>
@@ -1923,27 +1931,27 @@
         <v>92</v>
       </c>
       <c r="E5" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="3">
-        <v>46000.0</v>
+        <v>46000</v>
       </c>
       <c r="H5" s="3">
-        <v>115000.0</v>
+        <v>115000</v>
       </c>
       <c r="I5" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J5" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>93</v>
@@ -1952,27 +1960,27 @@
         <v>94</v>
       </c>
       <c r="E6" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="3">
-        <v>20000.0</v>
+        <v>20000</v>
       </c>
       <c r="H6" s="3">
-        <v>60000.0</v>
+        <v>60000</v>
       </c>
       <c r="I6" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J6" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>95</v>
@@ -1981,27 +1989,27 @@
         <v>96</v>
       </c>
       <c r="E7" s="2">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="3">
-        <v>28000.0</v>
+        <v>28000</v>
       </c>
       <c r="H7" s="3">
-        <v>64000.0</v>
+        <v>64000</v>
       </c>
       <c r="I7" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J7" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>97</v>
@@ -2010,27 +2018,27 @@
         <v>98</v>
       </c>
       <c r="E8" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="3">
-        <v>25000.0</v>
+        <v>25000</v>
       </c>
       <c r="H8" s="3">
-        <v>54000.0</v>
+        <v>54000</v>
       </c>
       <c r="I8" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J8" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="10">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>99</v>
@@ -2039,27 +2047,27 @@
         <v>100</v>
       </c>
       <c r="E9" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>26</v>
       </c>
       <c r="G9" s="3">
-        <v>20000.0</v>
+        <v>20000</v>
       </c>
       <c r="H9" s="3">
-        <v>49000.0</v>
+        <v>49000</v>
       </c>
       <c r="I9" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J9" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="10">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>101</v>
@@ -2068,27 +2076,27 @@
         <v>102</v>
       </c>
       <c r="E10" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>29</v>
       </c>
       <c r="G10" s="3">
-        <v>89000.0</v>
+        <v>89000</v>
       </c>
       <c r="H10" s="3">
-        <v>299000.0</v>
+        <v>299000</v>
       </c>
       <c r="I10" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J10" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="10">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>103</v>
@@ -2097,27 +2105,27 @@
         <v>104</v>
       </c>
       <c r="E11" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>32</v>
       </c>
       <c r="G11" s="3">
-        <v>51000.0</v>
+        <v>51000</v>
       </c>
       <c r="H11" s="3">
-        <v>112000.0</v>
+        <v>112000</v>
       </c>
       <c r="I11" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J11" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>105</v>
@@ -2126,27 +2134,27 @@
         <v>106</v>
       </c>
       <c r="E12" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="3">
-        <v>18000.0</v>
+        <v>18000</v>
       </c>
       <c r="H12" s="3">
-        <v>42000.0</v>
+        <v>42000</v>
       </c>
       <c r="I12" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J12" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>107</v>
@@ -2155,27 +2163,27 @@
         <v>108</v>
       </c>
       <c r="E13" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="3">
-        <v>48000.0</v>
+        <v>48000</v>
       </c>
       <c r="H13" s="3">
-        <v>120000.0</v>
+        <v>120000</v>
       </c>
       <c r="I13" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J13" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>109</v>
@@ -2184,27 +2192,27 @@
         <v>110</v>
       </c>
       <c r="E14" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>20</v>
       </c>
       <c r="G14" s="3">
-        <v>35000.0</v>
+        <v>35000</v>
       </c>
       <c r="H14" s="3">
-        <v>62000.0</v>
+        <v>62000</v>
       </c>
       <c r="I14" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J14" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="10">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>111</v>
@@ -2213,27 +2221,27 @@
         <v>92</v>
       </c>
       <c r="E15" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>17</v>
       </c>
       <c r="G15" s="3">
-        <v>34000.0</v>
+        <v>34000</v>
       </c>
       <c r="H15" s="3">
-        <v>80000.0</v>
+        <v>80000</v>
       </c>
       <c r="I15" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J15" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="10">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>112</v>
@@ -2242,27 +2250,27 @@
         <v>113</v>
       </c>
       <c r="E16" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G16" s="3">
-        <v>30000.0</v>
+        <v>30000</v>
       </c>
       <c r="H16" s="3">
-        <v>75000.0</v>
+        <v>75000</v>
       </c>
       <c r="I16" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J16" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="10">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>114</v>
@@ -2271,27 +2279,27 @@
         <v>115</v>
       </c>
       <c r="E17" s="2">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="3">
-        <v>40000.0</v>
+        <v>40000</v>
       </c>
       <c r="H17" s="3">
-        <v>93000.0</v>
+        <v>93000</v>
       </c>
       <c r="I17" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J17" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>116</v>
@@ -2300,27 +2308,27 @@
         <v>117</v>
       </c>
       <c r="E18" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>48</v>
       </c>
       <c r="G18" s="3">
-        <v>69000.0</v>
+        <v>69000</v>
       </c>
       <c r="H18" s="3">
-        <v>173000.0</v>
+        <v>173000</v>
       </c>
       <c r="I18" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J18" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="10">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>118</v>
@@ -2329,27 +2337,27 @@
         <v>119</v>
       </c>
       <c r="E19" s="6">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>51</v>
       </c>
       <c r="G19" s="3">
-        <v>20000.0</v>
+        <v>20000</v>
       </c>
       <c r="H19" s="3">
-        <v>49000.0</v>
+        <v>49000</v>
       </c>
       <c r="I19" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J19" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="10">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>120</v>
@@ -2358,27 +2366,27 @@
         <v>121</v>
       </c>
       <c r="E20" s="2">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>48</v>
       </c>
       <c r="G20" s="3">
-        <v>69000.0</v>
+        <v>69000</v>
       </c>
       <c r="H20" s="3">
-        <v>133000.0</v>
+        <v>133000</v>
       </c>
       <c r="I20" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J20" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="10">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>122</v>
@@ -2387,27 +2395,27 @@
         <v>123</v>
       </c>
       <c r="E21" s="2">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>32</v>
       </c>
       <c r="G21" s="3">
-        <v>67000.0</v>
+        <v>67000</v>
       </c>
       <c r="H21" s="3">
-        <v>103000.0</v>
+        <v>103000</v>
       </c>
       <c r="I21" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J21" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="10">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>124</v>
@@ -2416,27 +2424,27 @@
         <v>125</v>
       </c>
       <c r="E22" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="3">
-        <v>34000.0</v>
+        <v>34000</v>
       </c>
       <c r="H22" s="3">
-        <v>76000.0</v>
+        <v>76000</v>
       </c>
       <c r="I22" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J22" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B23" s="10">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>126</v>
@@ -2445,27 +2453,27 @@
         <v>127</v>
       </c>
       <c r="E23" s="2">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G23" s="3">
-        <v>101000.0</v>
+        <v>101000</v>
       </c>
       <c r="H23" s="3">
-        <v>182000.0</v>
+        <v>182000</v>
       </c>
       <c r="I23" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J23" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B24" s="10">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>128</v>
@@ -2474,25 +2482,25 @@
         <v>129</v>
       </c>
       <c r="E24" s="2">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>23</v>
       </c>
       <c r="G24" s="3">
-        <v>35000.0</v>
+        <v>35000</v>
       </c>
       <c r="H24" s="3">
-        <v>79000.0</v>
+        <v>79000</v>
       </c>
       <c r="I24" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="J24" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[19127478] count book, out of stock
</commit_message>
<xml_diff>
--- a/BookStore/window_data.xlsx
+++ b/BookStore/window_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\project 1\BookStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AA8A96-6E03-4661-AFDF-70A59A3799EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01CB653-0C74-4466-A260-9CEBF6F8FEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Short Story" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="173">
   <si>
     <t>ID</t>
   </si>
@@ -60,12 +60,6 @@
     <t>A CRAZY MIND</t>
   </si>
   <si>
-    <t>Hỉ Dương Tử</t>
-  </si>
-  <si>
-    <t>Trí</t>
-  </si>
-  <si>
     <t>Geulbaewoo</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>Jeffrey Archer</t>
   </si>
   <si>
-    <t>Ở Đây Zui Nè</t>
-  </si>
-  <si>
     <t>Tim Marshall</t>
   </si>
   <si>
@@ -544,6 +535,12 @@
   </si>
   <si>
     <t>Images/3_21.jpg</t>
+  </si>
+  <si>
+    <t>Hi Duong Tu</t>
+  </si>
+  <si>
+    <t>O Day Zui Ne</t>
   </si>
 </sst>
 </file>
@@ -845,8 +842,8 @@
   </sheetPr>
   <dimension ref="B3:J25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -892,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
@@ -901,7 +898,7 @@
         <v>1988</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G4" s="6">
         <v>20000</v>
@@ -921,7 +918,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
@@ -930,7 +927,7 @@
         <v>2021</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G5" s="6">
         <v>250000</v>
@@ -950,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -959,7 +956,7 @@
         <v>2021</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G6" s="6">
         <v>20000</v>
@@ -979,16 +976,16 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="E7" s="1">
         <v>2022</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G7" s="6">
         <v>35000</v>
@@ -1008,16 +1005,16 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="E8" s="1">
         <v>2020</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G8" s="6">
         <v>32000</v>
@@ -1037,16 +1034,16 @@
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E9" s="1">
         <v>2020</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G9" s="6">
         <v>41000</v>
@@ -1066,16 +1063,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1">
         <v>2020</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G10" s="6">
         <v>28000</v>
@@ -1095,16 +1092,16 @@
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E11" s="1">
         <v>2021</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G11" s="6">
         <v>50000</v>
@@ -1124,16 +1121,16 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1">
         <v>2020</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G12" s="6">
         <v>31000</v>
@@ -1153,16 +1150,16 @@
         <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E13" s="1">
         <v>2020</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G13" s="6">
         <v>16000</v>
@@ -1182,16 +1179,16 @@
         <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1">
         <v>2021</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G14" s="6">
         <v>87000</v>
@@ -1211,16 +1208,16 @@
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E15" s="1">
         <v>2020</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G15" s="6">
         <v>43000</v>
@@ -1240,16 +1237,16 @@
         <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E16" s="1">
         <v>2021</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G16" s="6">
         <v>36000</v>
@@ -1269,16 +1266,16 @@
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E17" s="1">
         <v>2020</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G17" s="6">
         <v>25000</v>
@@ -1298,16 +1295,16 @@
         <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E18" s="1">
         <v>2021</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G18" s="6">
         <v>26000</v>
@@ -1327,16 +1324,16 @@
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E19" s="5">
         <v>2018</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G19" s="6">
         <v>47000</v>
@@ -1356,16 +1353,16 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E20" s="1">
         <v>2018</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G20" s="6">
         <v>49000</v>
@@ -1385,16 +1382,16 @@
         <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E21" s="1">
         <v>2018</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G21" s="6">
         <v>37000</v>
@@ -1414,16 +1411,16 @@
         <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>21</v>
+        <v>172</v>
       </c>
       <c r="E22" s="1">
         <v>2021</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G22" s="6">
         <v>27000</v>
@@ -1443,16 +1440,16 @@
         <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E23" s="1">
         <v>2021</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G23" s="6">
         <v>38000</v>
@@ -1472,16 +1469,16 @@
         <v>21</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E24" s="1">
         <v>2017</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G24" s="6">
         <v>67000</v>
@@ -1501,16 +1498,16 @@
         <v>22</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E25" s="1">
         <v>2020</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G25" s="6">
         <v>128000</v>
@@ -1585,16 +1582,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1">
         <v>1988</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G4" s="6">
         <v>35000</v>
@@ -1614,16 +1611,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1">
         <v>2021</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G5" s="6">
         <v>20000</v>
@@ -1643,16 +1640,16 @@
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1">
         <v>2021</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G6" s="6">
         <v>42000</v>
@@ -1672,16 +1669,16 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1">
         <v>2022</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G7" s="6">
         <v>80000</v>
@@ -1701,16 +1698,16 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1">
         <v>2020</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G8" s="6">
         <v>28000</v>
@@ -1730,16 +1727,16 @@
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1">
         <v>2020</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G9" s="6">
         <v>46000</v>
@@ -1759,16 +1756,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E10" s="1">
         <v>2020</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G10" s="6">
         <v>31000</v>
@@ -1788,16 +1785,16 @@
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E11" s="1">
         <v>2021</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G11" s="6">
         <v>43000</v>
@@ -1817,16 +1814,16 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E12" s="1">
         <v>2020</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G12" s="6">
         <v>34000</v>
@@ -1846,16 +1843,16 @@
         <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E13" s="1">
         <v>2020</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G13" s="6">
         <v>37000</v>
@@ -1875,16 +1872,16 @@
         <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E14" s="1">
         <v>2021</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G14" s="6">
         <v>24000</v>
@@ -1904,16 +1901,16 @@
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E15" s="1">
         <v>2020</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G15" s="6">
         <v>30000</v>
@@ -1933,16 +1930,16 @@
         <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E16" s="1">
         <v>2021</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G16" s="6">
         <v>39000</v>
@@ -1969,7 +1966,7 @@
   </sheetPr>
   <dimension ref="B3:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -2016,16 +2013,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1">
         <v>1988</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G4" s="6">
         <v>25000</v>
@@ -2045,16 +2042,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E5" s="1">
         <v>2021</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G5" s="6">
         <v>46000</v>
@@ -2074,16 +2071,16 @@
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E6" s="1">
         <v>2021</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G6" s="6">
         <v>20000</v>
@@ -2103,16 +2100,16 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E7" s="1">
         <v>2022</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G7" s="6">
         <v>28000</v>
@@ -2132,16 +2129,16 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1">
         <v>2020</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G8" s="6">
         <v>25000</v>
@@ -2161,16 +2158,16 @@
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E9" s="1">
         <v>2020</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G9" s="6">
         <v>20000</v>
@@ -2190,16 +2187,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E10" s="1">
         <v>2020</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G10" s="6">
         <v>89000</v>
@@ -2219,16 +2216,16 @@
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E11" s="1">
         <v>2021</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G11" s="6">
         <v>51000</v>
@@ -2248,16 +2245,16 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1">
         <v>2020</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G12" s="6">
         <v>18000</v>
@@ -2277,16 +2274,16 @@
         <v>10</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1">
         <v>2020</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G13" s="6">
         <v>48000</v>
@@ -2306,16 +2303,16 @@
         <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E14" s="1">
         <v>2021</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G14" s="6">
         <v>35000</v>
@@ -2335,16 +2332,16 @@
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E15" s="1">
         <v>2020</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G15" s="6">
         <v>34000</v>
@@ -2364,16 +2361,16 @@
         <v>13</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E16" s="1">
         <v>2021</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G16" s="6">
         <v>30000</v>
@@ -2393,16 +2390,16 @@
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E17" s="1">
         <v>2020</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G17" s="6">
         <v>40000</v>
@@ -2422,16 +2419,16 @@
         <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E18" s="1">
         <v>2021</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G18" s="6">
         <v>69000</v>
@@ -2451,16 +2448,16 @@
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E19" s="5">
         <v>2018</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G19" s="6">
         <v>20000</v>
@@ -2480,16 +2477,16 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E20" s="1">
         <v>2018</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G20" s="6">
         <v>69000</v>
@@ -2509,16 +2506,16 @@
         <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E21" s="1">
         <v>2018</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G21" s="6">
         <v>67000</v>
@@ -2538,16 +2535,16 @@
         <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E22" s="1">
         <v>2021</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G22" s="6">
         <v>34000</v>
@@ -2567,16 +2564,16 @@
         <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E23" s="1">
         <v>2021</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G23" s="6">
         <v>101000</v>
@@ -2596,16 +2593,16 @@
         <v>21</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E24" s="1">
         <v>2017</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G24" s="6">
         <v>35000</v>

</xml_diff>

<commit_message>
[1927208] Fix minor bugs. Push all
</commit_message>
<xml_diff>
--- a/BookStore/window_data.xlsx
+++ b/BookStore/window_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\project 1\BookStore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ky Luong\Documents\GitHub\Project01_BookStore\BookStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01CB653-0C74-4466-A260-9CEBF6F8FEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AECF86-7C97-4445-9366-59ADFA972CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5190" yWindow="2100" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Short Story" sheetId="1" r:id="rId1"/>
@@ -498,9 +498,6 @@
     <t>Images/3_8.jpg</t>
   </si>
   <si>
-    <t>Images/3_9.jpg</t>
-  </si>
-  <si>
     <t>Images/3_10.jpg</t>
   </si>
   <si>
@@ -525,22 +522,25 @@
     <t>Images/3_17.jpg</t>
   </si>
   <si>
-    <t>Images/3_18.jpg</t>
-  </si>
-  <si>
-    <t>Images/3_19.jpg</t>
-  </si>
-  <si>
     <t>Images/3_20.jpg</t>
   </si>
   <si>
-    <t>Images/3_21.jpg</t>
-  </si>
-  <si>
     <t>Hi Duong Tu</t>
   </si>
   <si>
     <t>O Day Zui Ne</t>
+  </si>
+  <si>
+    <t>Images/3_18.png</t>
+  </si>
+  <si>
+    <t>Images/3_19.png</t>
+  </si>
+  <si>
+    <t>Images/3_21.png</t>
+  </si>
+  <si>
+    <t>Images/3_9.png</t>
   </si>
 </sst>
 </file>
@@ -842,20 +842,20 @@
   </sheetPr>
   <dimension ref="B3:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="58.21875" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -884,7 +884,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -913,7 +913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -942,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -971,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -979,7 +979,7 @@
         <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E7" s="1">
         <v>2022</v>
@@ -1000,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>7</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>8</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>9</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>10</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>11</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>12</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>13</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>14</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>15</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>16</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>17</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>18</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>19</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>53</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E22" s="1">
         <v>2021</v>
@@ -1435,7 +1435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>20</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>21</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>22</v>
       </c>
@@ -1536,19 +1536,19 @@
   <dimension ref="B3:J16"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="61.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="61.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="14.77734375" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>1</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>2</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>3</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>4</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>5</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>6</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>7</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>8</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>9</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>10</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>11</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>12</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>13</v>
       </c>
@@ -1966,20 +1966,20 @@
   </sheetPr>
   <dimension ref="B3:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="53.5546875" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>1</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>2</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>3</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>4</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>5</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>6</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>7</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>8</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>9</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>2020</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="G12" s="6">
         <v>18000</v>
@@ -2269,7 +2269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>10</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>2020</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G13" s="6">
         <v>48000</v>
@@ -2298,7 +2298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>11</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>2021</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G14" s="6">
         <v>35000</v>
@@ -2327,7 +2327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>12</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>2020</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G15" s="6">
         <v>34000</v>
@@ -2356,7 +2356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>13</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>2021</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G16" s="6">
         <v>30000</v>
@@ -2385,7 +2385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <v>14</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>2020</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G17" s="6">
         <v>40000</v>
@@ -2414,7 +2414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <v>15</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>2021</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G18" s="6">
         <v>69000</v>
@@ -2443,7 +2443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
         <v>16</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>2018</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G19" s="6">
         <v>20000</v>
@@ -2472,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <v>17</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>2018</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G20" s="6">
         <v>69000</v>
@@ -2501,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
         <v>18</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>2018</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G21" s="6">
         <v>67000</v>
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
         <v>19</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>2021</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G22" s="6">
         <v>34000</v>
@@ -2559,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
         <v>20</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>2021</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G23" s="6">
         <v>101000</v>
@@ -2588,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
         <v>21</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>2017</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G24" s="6">
         <v>35000</v>

</xml_diff>